<commit_message>
Fixed the @ issue while running all tests, Added extent reports system info, Changed the action class driver
</commit_message>
<xml_diff>
--- a/magento_data/test_data.xlsx
+++ b/magento_data/test_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -59,6 +59,21 @@
     <t>qty</t>
   </si>
   <si>
+    <t>street_address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>post_code</t>
+  </si>
+  <si>
     <t>Vinay</t>
   </si>
   <si>
@@ -87,6 +102,15 @@
   </si>
   <si>
     <t>Montana Wind Jacket</t>
+  </si>
+  <si>
+    <t>Bettappa Road, 2nd Cross</t>
+  </si>
+  <si>
+    <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>IN</t>
   </si>
   <si>
     <t>thundurustest@gmail.com</t>
@@ -100,10 +124,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -126,11 +150,102 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -139,15 +254,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,44 +262,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -204,73 +290,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -283,49 +307,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -337,133 +487,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,7 +505,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,61 +551,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,140 +574,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1046,10 +1070,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -1061,7 +1085,7 @@
     <col min="1033" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1104,93 +1128,138 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" spans="1:14">
+    <row r="2" ht="15.75" spans="1:19">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2">
         <v>9945723812</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="N2" s="2">
         <v>1</v>
       </c>
+      <c r="O2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>549</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="2">
+        <v>560070</v>
+      </c>
     </row>
-    <row r="3" ht="31.5" spans="1:14">
+    <row r="3" ht="31.5" spans="1:19">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H3" s="2">
         <v>9945723812</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="N3" s="2">
         <v>1</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>549</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="2">
+        <v>560070</v>
       </c>
     </row>
   </sheetData>

</xml_diff>